<commit_message>
Mixed results, not negative change.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_naplan_uploader/education_naplan.xlsx
+++ b/dashboard_loader/education_naplan_uploader/education_naplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" state="visible" r:id="rId2"/>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative change</t>
+    <t xml:space="preserve">Mixed results</t>
   </si>
   <si>
     <t xml:space="preserve">Updated</t>
@@ -264,7 +264,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A34"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1379,7 +1379,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A34"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2572,7 +2572,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A34"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3730,8 +3730,8 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4845,8 +4845,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="A3:A34 B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>